<commit_message>
Alterado o nome das abas das planilhas.
</commit_message>
<xml_diff>
--- a/Batch/CreateBase/Files/Estado.xlsx
+++ b/Batch/CreateBase/Files/Estado.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\CepBrasil\App\Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/75c94e6676613aaf/Projetos/Exkyn.Cep/Batch/CreateBase/Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DA132E1-ADB7-4383-8124-AEFCD296FFCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{4DA132E1-ADB7-4383-8124-AEFCD296FFCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A44E0311-AE20-4EAF-95E4-1A05418B4B83}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Estado" sheetId="1" r:id="rId1"/>
+    <sheet name="States" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -1037,12 +1037,12 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>54</v>
       </c>
@@ -1053,7 +1053,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1064,7 +1064,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1075,7 +1075,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1086,7 +1086,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1097,7 +1097,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1108,7 +1108,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1119,7 +1119,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1130,7 +1130,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1141,7 +1141,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1152,7 +1152,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1163,7 +1163,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1174,7 +1174,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1185,7 +1185,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1196,7 +1196,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1207,7 +1207,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1218,7 +1218,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1229,7 +1229,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1240,7 +1240,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1251,7 +1251,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1262,7 +1262,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1273,7 +1273,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1284,7 +1284,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1295,7 +1295,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1306,7 +1306,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1317,7 +1317,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1328,7 +1328,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1339,7 +1339,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>

</xml_diff>